<commit_message>
The application is running, I included instructions how to use the user interface and I updated the excel sheet with project information
</commit_message>
<xml_diff>
--- a/ProjectManagement/TasksOrganizer_General_Info.xlsx
+++ b/ProjectManagement/TasksOrganizer_General_Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fjerena\Documents\Project TasksOrganizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fjerena\Documents\Project TasksOrganizer\TasksOrganizer\ProjectManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7D8D77-076D-4CA9-9AC9-7A47A7F7E0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB69E346-C5BB-4F75-86C6-7E36EEAFAFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15045" yWindow="-18165" windowWidth="29040" windowHeight="17640" xr2:uid="{1310EBEC-0004-418C-8810-4BC9F39BDC58}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1310EBEC-0004-418C-8810-4BC9F39BDC58}"/>
   </bookViews>
   <sheets>
     <sheet name="WeightMatrix" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
   <si>
     <t>Very_Low</t>
   </si>
@@ -277,6 +277,9 @@
 how to work in GITHUB
 - The main discussion will be about productivity and how to organize your tasks
 - Include Pareto´s distribution in my text</t>
+  </si>
+  <si>
+    <t>Convert the application to .exe file, that can be executed on the local PC without to have Python installed</t>
   </si>
 </sst>
 </file>
@@ -367,12 +370,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -382,9 +382,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -393,13 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -431,9 +422,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -471,7 +462,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -577,7 +568,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -719,7 +710,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -757,35 +748,35 @@
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="11">
         <v>0.6</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="17" t="s">
+      <c r="O14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
     </row>
     <row r="15" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="10">
         <f>1-B14</f>
         <v>0.4</v>
       </c>
@@ -865,7 +856,7 @@
       </c>
     </row>
     <row r="17" spans="3:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -894,7 +885,7 @@
         <f t="shared" si="0"/>
         <v>3.8000000000000003</v>
       </c>
-      <c r="L17" s="16" t="s">
+      <c r="L17" s="12" t="s">
         <v>9</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -925,7 +916,7 @@
       </c>
     </row>
     <row r="18" spans="3:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="16"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="2" t="s">
         <v>1</v>
       </c>
@@ -952,7 +943,7 @@
         <f t="shared" si="2"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="L18" s="16"/>
+      <c r="L18" s="12"/>
       <c r="M18" s="2" t="s">
         <v>1</v>
       </c>
@@ -981,7 +972,7 @@
       </c>
     </row>
     <row r="19" spans="3:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="16"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="2" t="s">
         <v>2</v>
       </c>
@@ -1008,7 +999,7 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="L19" s="16"/>
+      <c r="L19" s="12"/>
       <c r="M19" s="2" t="s">
         <v>2</v>
       </c>
@@ -1037,7 +1028,7 @@
       </c>
     </row>
     <row r="20" spans="3:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="16"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1064,7 +1055,7 @@
         <f t="shared" si="2"/>
         <v>6.2</v>
       </c>
-      <c r="L20" s="16"/>
+      <c r="L20" s="12"/>
       <c r="M20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1093,7 +1084,7 @@
       </c>
     </row>
     <row r="21" spans="3:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="16"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1120,7 +1111,7 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="L21" s="16"/>
+      <c r="L21" s="12"/>
       <c r="M21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1155,14 +1146,14 @@
       </c>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C25" s="4"/>
-      <c r="D25" s="5" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C26" s="6"/>
-      <c r="D26" s="5" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1173,8 +1164,8 @@
     <mergeCell ref="O14:S14"/>
     <mergeCell ref="L17:L21"/>
   </mergeCells>
-  <conditionalFormatting sqref="O17:S21">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="F17:J21">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1185,8 +1176,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17:J21">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="O17:S21">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1206,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353D6114-59EB-4496-84B9-1E8385F8D897}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1220,193 +1211,197 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="11" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="11" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
-        <v>5</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
-        <v>11</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
-        <v>13</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="11">
-        <v>15</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="11">
-        <v>16</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
-        <v>17</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
-        <v>19</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
-        <v>20</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1418,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6EA9C2-2BD8-46CF-B3EF-1FE1181D4513}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,204 +1425,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>11</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>13</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>14</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>6</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="3" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>7</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
-        <v>7</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="3" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>9</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
-        <v>8</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="3" t="s">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
-        <v>9</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="3" t="s">
+    <row r="16" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
-        <v>10</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
-        <v>12</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
-        <v>15</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="13">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1653,66 +1648,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>